<commit_message>
refactor:build: Refatorando App, criando backend e frontend/ instalando dependencias de documentação
</commit_message>
<xml_diff>
--- a/data/planilha_vendas.xlsx
+++ b/data/planilha_vendas.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet r:id="rId1" sheetId="1" name="Página1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -85,22 +88,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="d.m"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,49 +112,77 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -177,22 +209,82 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -204,424 +296,458 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.13"/>
+    <col min="1" max="1" style="6" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>45292.0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="1">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
         <v>1.14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>45293.0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>45432.0</v>
+        <v>45293</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>37.1</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>45294.0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D4" s="1">
+        <v>45294</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5">
         <v>38.5</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>45295.0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>10.0</v>
+        <v>45295</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>45296.0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D6" s="1">
+        <v>45296</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
         <v>15.5</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>45297.0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="D7" s="1">
+        <v>45297</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5">
         <v>201.1</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2">
-        <v>45298.0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2132.0</v>
+        <v>45298</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2132</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2">
-        <v>45299.0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>20.0</v>
+        <v>45299</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>45300.0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="D10" s="1">
+        <v>45300</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5">
         <v>13.2</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2">
-        <v>45301.0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="D11" s="1">
+        <v>45301</v>
+      </c>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
         <v>33.12</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2">
-        <v>45302.0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="D12" s="1">
+        <v>45302</v>
+      </c>
+      <c r="C12" s="4">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5">
         <v>44.25</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2">
-        <v>45303.0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="D13" s="1">
+        <v>45303</v>
+      </c>
+      <c r="C13" s="4">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5">
         <v>38.5</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="2">
-        <v>45304.0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>20.0</v>
+        <v>45304</v>
+      </c>
+      <c r="C14" s="4">
+        <v>13</v>
+      </c>
+      <c r="D14" s="4">
+        <v>20</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2">
-        <v>45305.0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="D15" s="1">
+        <v>45305</v>
+      </c>
+      <c r="C15" s="4">
+        <v>14</v>
+      </c>
+      <c r="D15" s="5">
         <v>201.1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="2">
-        <v>45306.0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>10.0</v>
+        <v>45306</v>
+      </c>
+      <c r="C16" s="4">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4">
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>